<commit_message>
excel 2015 à jour
</commit_message>
<xml_diff>
--- a/excel/coildict.xlsx
+++ b/excel/coildict.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-18920" windowWidth="21600" windowHeight="38400"/>
+    <workbookView xWindow="2000" yWindow="460" windowWidth="21600" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$40</definedName>
+  </definedNames>
   <calcPr calcId="150001" calcMode="autoNoTable" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>endsec</t>
   </si>
@@ -174,15 +177,35 @@
   </si>
   <si>
     <t>end2</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -219,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,35 +265,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -574,864 +590,1059 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A30" activeCellId="2" sqref="A11:XFD11 A22:XFD22 A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="15.1640625" style="1"/>
+    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
         <v>89</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
         <v>66</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>127</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>55</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>70</v>
       </c>
-      <c r="H3" s="1">
-        <f>INT($B3*10/9+D3)</f>
+      <c r="I3" s="1">
+        <f>INT($C3*10/9+E3)</f>
         <v>128</v>
       </c>
-      <c r="I3" s="1">
-        <f>INT($B3*10/9+E3)</f>
+      <c r="J3" s="1">
+        <f>INT($C3*10/9+F3)</f>
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
         <v>83</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>108</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>60</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>78</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:I40" si="0">INT($B4*10/9+D4)</f>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:J34" si="0">INT($C4*10/9+E4)</f>
         <v>152</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>224</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>271</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
-        <f>C5-B5</f>
+      <c r="F5" s="1">
+        <f>D5-C5</f>
         <v>47</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>248</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <f t="shared" si="0"/>
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>49</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>171</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" ref="E6:E9" si="1">C6-B6</f>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6:F9" si="1">D6-C6</f>
         <v>122</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <f t="shared" si="0"/>
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>51</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>83</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>221</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>228</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
         <v>245</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>23</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>26</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>12</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>21</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>89</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>29</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>48</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>52</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>62</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>28</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>70</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>90</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>110</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
-      <c r="J11" s="1">
-        <f t="shared" ref="J4:J34" si="2">$B11+F11</f>
+      <c r="K11" s="1">
+        <f t="shared" ref="K11:K30" si="2">$C11+G11</f>
         <v>142</v>
       </c>
-      <c r="K11" s="1">
-        <f t="shared" ref="K4:K34" si="3">$B11+G11</f>
+      <c r="L11" s="1">
+        <f t="shared" ref="L11:L30" si="3">$C11+H11</f>
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>227</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>314</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>71</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>81</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>112</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>20</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>50</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>253</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>294</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>45</v>
       </c>
-      <c r="E15" s="1">
-        <f>C15-B15</f>
+      <c r="F15" s="1">
+        <f>D15-C15</f>
         <v>41</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <f t="shared" si="0"/>
         <v>326</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <f t="shared" si="0"/>
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>94</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>149</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>13</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>68</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <f t="shared" si="0"/>
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>68</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>120</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>15</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>32</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>225</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>72</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>90</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>8</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>28</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>66</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>88</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>10</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>40</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>65</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>126</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>5</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>120</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>40</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>8</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>111</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>26</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>50</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>100</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>43</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>16</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>44</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="1">
         <v>77</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>88</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>0</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>60</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>50</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>23</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>103</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>60</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>100</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>52</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>90</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>109</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>15</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>32</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <f t="shared" si="0"/>
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>53</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>91</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>56</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>177</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>62</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29" s="1">
         <v>54</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>65</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30" s="1">
         <v>101</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>196</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>20</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>80</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>100</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>130</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <f t="shared" si="0"/>
         <v>132</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <f t="shared" si="2"/>
         <v>201</v>
       </c>
-      <c r="K30" s="1">
+      <c r="L30" s="1">
         <f t="shared" si="3"/>
         <v>231</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>66</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="1">
         <v>70</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>71</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32" s="1">
         <v>141</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>303</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>20</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>120</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <f t="shared" si="0"/>
         <v>176</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <f t="shared" si="0"/>
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>72</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" s="1">
         <v>16</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>126</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>30</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>90</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>74</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="1">
+      <c r="C34" s="1">
         <v>84</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>135</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>15</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>80</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <f t="shared" si="0"/>
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>78</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C35" s="1">
         <v>52</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>79</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="1">
+      <c r="C36" s="1">
         <v>79</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>80</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="1">
+      <c r="C37" s="1">
         <v>75</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>81</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="1">
+      <c r="C38" s="1">
         <v>33</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>82</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="1">
         <v>13</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>83</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>59</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>111</v>
       </c>
     </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="5"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:L40">
+    <filterColumn colId="8">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>